<commit_message>
Firmware Atmega16 Update (Clock Fix)
Bug Fixes
</commit_message>
<xml_diff>
--- a/Datasheets-Libs/Lixie-Uhr-Bestellliste.xlsx
+++ b/Datasheets-Libs/Lixie-Uhr-Bestellliste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erena\OneDrive\Dokumente\GitHub\lixie\Datasheets-Libs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samir El-Farfar\Documents\GitHub\lixie\Datasheets-Libs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413DB8C0-4627-4968-8EF0-A5E8B66C35E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A8F6BD-5B2E-4142-90F3-5B980DB8F744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -808,7 +808,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="56">
+  <fills count="57">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1101,6 +1101,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1491,7 +1497,7 @@
     <xf numFmtId="0" fontId="40" fillId="54" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1676,6 +1682,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="56" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="85">
@@ -2243,27 +2252,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="5.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="29.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="10" style="3" customWidth="1"/>
     <col min="7" max="7" width="19" style="3" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" style="41" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="44"/>
-    <col min="12" max="16384" width="11.42578125" style="2"/>
+    <col min="8" max="8" width="6.109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="21.88671875" style="41" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" style="44"/>
+    <col min="12" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>28</v>
       </c>
@@ -2279,7 +2288,7 @@
       </c>
       <c r="J1" s="37"/>
     </row>
-    <row r="2" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21"/>
       <c r="B2" s="17"/>
       <c r="C2" s="18"/>
@@ -2293,7 +2302,7 @@
       </c>
       <c r="J2" s="37"/>
     </row>
-    <row r="3" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="66" t="s">
         <v>62</v>
       </c>
@@ -2310,7 +2319,7 @@
       <c r="I3" s="63"/>
       <c r="J3" s="38"/>
     </row>
-    <row r="4" spans="1:11" s="7" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" s="7" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -2343,7 +2352,7 @@
       </c>
       <c r="K4" s="45"/>
     </row>
-    <row r="5" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="64" t="s">
         <v>12</v>
       </c>
@@ -2358,7 +2367,7 @@
       <c r="J5" s="65"/>
       <c r="K5" s="45"/>
     </row>
-    <row r="6" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="1"/>
       <c r="C6" s="13"/>
@@ -2373,7 +2382,7 @@
       </c>
       <c r="J6" s="35"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="64" t="s">
         <v>13</v>
       </c>
@@ -2387,7 +2396,7 @@
       <c r="I7" s="65"/>
       <c r="J7" s="65"/>
     </row>
-    <row r="8" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>2</v>
       </c>
@@ -2419,7 +2428,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="66" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>3</v>
       </c>
@@ -2451,7 +2460,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>4</v>
       </c>
@@ -2483,7 +2492,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>5</v>
       </c>
@@ -2515,7 +2524,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="64" t="s">
         <v>14</v>
       </c>
@@ -2529,7 +2538,7 @@
       <c r="I12" s="65"/>
       <c r="J12" s="65"/>
     </row>
-    <row r="13" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="58" t="s">
         <v>15</v>
       </c>
@@ -2543,7 +2552,7 @@
       <c r="I13" s="59"/>
       <c r="J13" s="60"/>
     </row>
-    <row r="15" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>29</v>
       </c>
@@ -2559,7 +2568,7 @@
       </c>
       <c r="J15" s="37"/>
     </row>
-    <row r="16" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A16" s="21"/>
       <c r="B16" s="17"/>
       <c r="C16" s="18"/>
@@ -2573,7 +2582,7 @@
       </c>
       <c r="J16" s="37"/>
     </row>
-    <row r="17" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A17" s="66" t="s">
         <v>64</v>
       </c>
@@ -2590,7 +2599,7 @@
       <c r="I17" s="63"/>
       <c r="J17" s="38"/>
     </row>
-    <row r="18" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>2</v>
       </c>
@@ -2622,7 +2631,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="64" t="s">
         <v>12</v>
       </c>
@@ -2636,7 +2645,7 @@
       <c r="I19" s="65"/>
       <c r="J19" s="65"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>1</v>
       </c>
@@ -2653,7 +2662,7 @@
       </c>
       <c r="J20" s="35"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="64" t="s">
         <v>13</v>
       </c>
@@ -2667,7 +2676,7 @@
       <c r="I21" s="65"/>
       <c r="J21" s="65"/>
     </row>
-    <row r="22" spans="1:11" ht="102" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>2</v>
       </c>
@@ -2677,7 +2686,7 @@
       <c r="C22" s="12">
         <v>1</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="69" t="s">
         <v>20</v>
       </c>
       <c r="E22" s="1" t="s">
@@ -2699,7 +2708,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>3</v>
       </c>
@@ -2731,7 +2740,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="66" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>4</v>
       </c>
@@ -2763,7 +2772,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>5</v>
       </c>
@@ -2798,7 +2807,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>6</v>
       </c>
@@ -2833,7 +2842,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>7</v>
       </c>
@@ -2868,7 +2877,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="66" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>8</v>
       </c>
@@ -2878,7 +2887,7 @@
       <c r="C28" s="12">
         <v>25</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="69" t="s">
         <v>52</v>
       </c>
       <c r="E28" s="32" t="s">
@@ -2900,7 +2909,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="66" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>9</v>
       </c>
@@ -2932,7 +2941,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>10</v>
       </c>
@@ -2967,7 +2976,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="66" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>11</v>
       </c>
@@ -3002,7 +3011,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="64" t="s">
         <v>14</v>
       </c>
@@ -3016,7 +3025,7 @@
       <c r="I32" s="65"/>
       <c r="J32" s="65"/>
     </row>
-    <row r="33" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="66" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>12</v>
       </c>
@@ -3048,7 +3057,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="58" t="s">
         <v>15</v>
       </c>
@@ -3062,7 +3071,7 @@
       <c r="I34" s="59"/>
       <c r="J34" s="60"/>
     </row>
-    <row r="37" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A37" s="16" t="s">
         <v>29</v>
       </c>
@@ -3078,7 +3087,7 @@
       </c>
       <c r="J37" s="37"/>
     </row>
-    <row r="38" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A38" s="21"/>
       <c r="B38" s="17"/>
       <c r="C38" s="18"/>
@@ -3092,7 +3101,7 @@
       </c>
       <c r="J38" s="37"/>
     </row>
-    <row r="39" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A39" s="31" t="s">
         <v>65</v>
       </c>
@@ -3109,7 +3118,7 @@
       <c r="I39" s="26"/>
       <c r="J39" s="38"/>
     </row>
-    <row r="40" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>2</v>
       </c>
@@ -3141,7 +3150,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="27" t="s">
         <v>36</v>
       </c>
@@ -3155,7 +3164,7 @@
       <c r="I41" s="28"/>
       <c r="J41" s="39"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>1</v>
       </c>
@@ -3178,7 +3187,7 @@
       </c>
       <c r="J42" s="35"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>2</v>
       </c>
@@ -3198,7 +3207,7 @@
       <c r="I43" s="10"/>
       <c r="J43" s="35"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>3</v>
       </c>
@@ -3216,7 +3225,7 @@
       <c r="I44" s="10"/>
       <c r="J44" s="35"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>4</v>
       </c>
@@ -3236,7 +3245,7 @@
       <c r="I45" s="10"/>
       <c r="J45" s="35"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="33" t="s">
         <v>15</v>
       </c>
@@ -3298,10 +3307,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -3312,10 +3322,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -3453,18 +3464,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3486,18 +3497,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{866A4294-3582-458B-9610-8F865127EDC3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A24FE4B-D46A-4FED-B08C-25D61171B1A1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{866A4294-3582-458B-9610-8F865127EDC3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>